<commit_message>
add result nie działa
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>Summary Report</t>
   </si>
@@ -29,19 +29,22 @@
     <t>Przemek</t>
   </si>
   <si>
+    <t xml:space="preserve">Podsumowanie: </t>
+  </si>
+  <si>
     <t>Podsumowanie:</t>
   </si>
   <si>
     <t>Gracze:</t>
   </si>
   <si>
-    <t>LiczbaMeczy:</t>
-  </si>
-  <si>
-    <t>LiczbaPiw:</t>
-  </si>
-  <si>
-    <t>LiczbaZetonow:</t>
+    <t>Podsumowanie Piw</t>
+  </si>
+  <si>
+    <t>Podsumowanie Punktów</t>
+  </si>
+  <si>
+    <t>Podsumowanie Żetonów</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,102 +391,279 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>1</v>
       </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>300</v>
       </c>
-      <c r="C5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>650</v>
+      </c>
+      <c r="C19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>200</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>1150</v>
+      </c>
+      <c r="C25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>20</v>
+      </c>
+      <c r="B26">
+        <v>200</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>1350</v>
+      </c>
+      <c r="C27">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>500</v>
-      </c>
-      <c r="C6">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
+      <c r="B31">
+        <f>B27</f>
+        <v>1350</v>
+      </c>
+      <c r="C31">
+        <v>1251</v>
+      </c>
+      <c r="D31">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B7">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>900</v>
-      </c>
-      <c r="E13">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>357</v>
-      </c>
-      <c r="E14">
-        <v>92</v>
+      <c r="B32">
+        <f>C27</f>
+        <v>610</v>
+      </c>
+      <c r="C32">
+        <v>604</v>
+      </c>
+      <c r="D32">
+        <v>1006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>